<commit_message>
add 3 first map
</commit_message>
<xml_diff>
--- a/ResultsTransformation/Map/Villes/bourg-palette.xlsx
+++ b/ResultsTransformation/Map/Villes/bourg-palette.xlsx
@@ -424,1071 +424,1071 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1513,24 +1513,24 @@
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1555,44 +1555,44 @@
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1617,32 +1617,32 @@
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>x</t>
         </is>
       </c>
     </row>

</xml_diff>